<commit_message>
Finished custom work on exporter codes special cases
</commit_message>
<xml_diff>
--- a/pyeconlab/trade/dataset/NBERFeenstraWTF/checks/check_exporters.xlsx
+++ b/pyeconlab/trade/dataset/NBERFeenstraWTF/checks/check_exporters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="16095" windowHeight="9600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="456">
   <si>
     <t>exporter</t>
   </si>
@@ -1353,29 +1353,56 @@
     <t>Encode as CHN, as per ISO3N</t>
   </si>
   <si>
-    <t>Italy!, Why isn't this in UN CountryList?</t>
-  </si>
-  <si>
     <t>Panama (before adding Panama Canal Zone in 1979)</t>
   </si>
   <si>
     <t>638 = Reunion</t>
   </si>
   <si>
-    <t>756 = Switzerland, Why doesn't UN Match this?</t>
-  </si>
-  <si>
-    <t>USA!, Why isn't this in UN CountryList?</t>
-  </si>
-  <si>
-    <t>158 Taiwan</t>
+    <t>250 = France. Is this Monaco, 492?</t>
   </si>
   <si>
     <t>Ethiopia used numeric code 230 before Eritrea split away in 1993 
-Should this be encoded as 231 which is the current code for Ethiopia OR 230 to 1993 and then 231 from 1994 to 2000?</t>
-  </si>
-  <si>
-    <t>250 = France. Is this Monaco, 492?</t>
+Should this be encoded as 231 which is the current code for Ethiopia OR 230 to 1993 and then 231 from 1994 to 2000? Eritrea = 232</t>
+  </si>
+  <si>
+    <t>Keep as 230 numerically</t>
+  </si>
+  <si>
+    <t>In CEPII and UN ITL is coded as 381</t>
+  </si>
+  <si>
+    <t>Recode as 381</t>
+  </si>
+  <si>
+    <t>Recode as 579</t>
+  </si>
+  <si>
+    <t>CEPII and UN have NOR as 579. Why is this different to WIKI (578)</t>
+  </si>
+  <si>
+    <t>757 = Switzerland, Why doesn't UN Match this?</t>
+  </si>
+  <si>
+    <t>Recode to 757</t>
+  </si>
+  <si>
+    <t>Recode to 842</t>
+  </si>
+  <si>
+    <t>USA!, Why isn't this in UN CountryList? 841 1962 to 1980; 842 1981 to 2061</t>
+  </si>
+  <si>
+    <t>UN Code is 882</t>
+  </si>
+  <si>
+    <t>158 Taiwan; CEPII is 490 as it is Asia, NES</t>
+  </si>
+  <si>
+    <t>Recode to 158, 'TWN'</t>
+  </si>
+  <si>
+    <t>Recode to 882, 'WSM'</t>
   </si>
 </sst>
 </file>
@@ -1782,8 +1809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
+      <selection activeCell="H189" sqref="H189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -2738,10 +2765,10 @@
         <v>428</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>435</v>
+        <v>443</v>
       </c>
       <c r="H54" s="12" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
@@ -2832,7 +2859,7 @@
         <v>435</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.35">
@@ -3344,8 +3371,11 @@
       <c r="F89" s="9" t="s">
         <v>427</v>
       </c>
+      <c r="G89" s="3" t="s">
+        <v>445</v>
+      </c>
       <c r="H89" s="2" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.35">
@@ -4027,6 +4057,12 @@
       <c r="F129" s="11" t="s">
         <v>432</v>
       </c>
+      <c r="G129" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="H129" s="2" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" s="5" t="s">
@@ -4062,7 +4098,7 @@
         <v>432</v>
       </c>
       <c r="H131" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.35">
@@ -4218,7 +4254,7 @@
         <v>432</v>
       </c>
       <c r="H140" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.35">
@@ -4611,8 +4647,11 @@
       <c r="F163" s="9" t="s">
         <v>427</v>
       </c>
+      <c r="G163" s="3" t="s">
+        <v>449</v>
+      </c>
       <c r="H163" s="2" t="s">
-        <v>442</v>
+        <v>448</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.35">
@@ -4904,10 +4943,10 @@
         <v>427</v>
       </c>
       <c r="G180" s="3" t="s">
-        <v>435</v>
+        <v>450</v>
       </c>
       <c r="H180" s="2" t="s">
-        <v>443</v>
+        <v>451</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.35">
@@ -5045,6 +5084,12 @@
       <c r="F188" s="11" t="s">
         <v>432</v>
       </c>
+      <c r="G188" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="H188" s="2" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A189" s="5" t="s">
@@ -5130,8 +5175,11 @@
       <c r="F193" s="9" t="s">
         <v>429</v>
       </c>
+      <c r="G193" s="3" t="s">
+        <v>454</v>
+      </c>
       <c r="H193" s="2" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Evening edits of country concord for NBERFeenstra
</commit_message>
<xml_diff>
--- a/pyeconlab/trade/dataset/NBERFeenstraWTF/checks/check_exporters.xlsx
+++ b/pyeconlab/trade/dataset/NBERFeenstraWTF/checks/check_exporters.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24816"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="16095" windowHeight="9600"/>
+    <workbookView xWindow="240" yWindow="80" windowWidth="16100" windowHeight="9600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1409,7 +1414,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1428,6 +1433,22 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1465,8 +1486,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1507,7 +1546,25 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="19">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1810,23 +1867,23 @@
   <dimension ref="A1:H202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="H189" sqref="H189"/>
+      <selection activeCell="F180" sqref="F180:H180"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="9.7109375" style="9" customWidth="1"/>
-    <col min="7" max="7" width="35.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="70.42578125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="2" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="2"/>
+    <col min="6" max="6" width="9.6640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="35.1640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="70.5" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1849,7 +1906,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1866,7 +1923,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
         <v>100</v>
       </c>
@@ -1889,7 +1946,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8">
       <c r="A4" s="5" t="s">
         <v>101</v>
       </c>
@@ -1909,7 +1966,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
         <v>141</v>
       </c>
@@ -1926,7 +1983,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -1943,7 +2000,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
@@ -1960,7 +2017,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
         <v>181</v>
       </c>
@@ -1977,7 +2034,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8">
       <c r="A9" s="5" t="s">
         <v>51</v>
       </c>
@@ -1994,7 +2051,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8">
       <c r="A10" s="5" t="s">
         <v>150</v>
       </c>
@@ -2011,7 +2068,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8">
       <c r="A11" s="5" t="s">
         <v>133</v>
       </c>
@@ -2028,7 +2085,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8">
       <c r="A12" s="5" t="s">
         <v>67</v>
       </c>
@@ -2045,7 +2102,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8">
       <c r="A13" s="5" t="s">
         <v>85</v>
       </c>
@@ -2062,7 +2119,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8">
       <c r="A14" s="5" t="s">
         <v>167</v>
       </c>
@@ -2079,7 +2136,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8">
       <c r="A15" s="5" t="s">
         <v>182</v>
       </c>
@@ -2096,7 +2153,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8">
       <c r="A16" s="5" t="s">
         <v>68</v>
       </c>
@@ -2113,7 +2170,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6">
       <c r="A17" s="5" t="s">
         <v>122</v>
       </c>
@@ -2130,7 +2187,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6">
       <c r="A18" s="5" t="s">
         <v>49</v>
       </c>
@@ -2147,7 +2204,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6">
       <c r="A19" s="5" t="s">
         <v>52</v>
       </c>
@@ -2164,7 +2221,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6">
       <c r="A20" s="5" t="s">
         <v>195</v>
       </c>
@@ -2181,7 +2238,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6">
       <c r="A21" s="5" t="s">
         <v>53</v>
       </c>
@@ -2198,7 +2255,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6">
       <c r="A22" s="5" t="s">
         <v>164</v>
       </c>
@@ -2215,7 +2272,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6">
       <c r="A23" s="5" t="s">
         <v>77</v>
       </c>
@@ -2232,7 +2289,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6">
       <c r="A24" s="5" t="s">
         <v>142</v>
       </c>
@@ -2249,7 +2306,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6">
       <c r="A25" s="5" t="s">
         <v>102</v>
       </c>
@@ -2266,7 +2323,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6">
       <c r="A26" s="5" t="s">
         <v>18</v>
       </c>
@@ -2283,7 +2340,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6">
       <c r="A27" s="5" t="s">
         <v>190</v>
       </c>
@@ -2300,7 +2357,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6">
       <c r="A28" s="5" t="s">
         <v>103</v>
       </c>
@@ -2317,7 +2374,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6">
       <c r="A29" s="5" t="s">
         <v>12</v>
       </c>
@@ -2334,7 +2391,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6">
       <c r="A30" s="5" t="s">
         <v>47</v>
       </c>
@@ -2351,7 +2408,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6">
       <c r="A31" s="5" t="s">
         <v>13</v>
       </c>
@@ -2368,7 +2425,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6">
       <c r="A32" s="5" t="s">
         <v>104</v>
       </c>
@@ -2385,7 +2442,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8">
       <c r="A33" s="5" t="s">
         <v>14</v>
       </c>
@@ -2402,7 +2459,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8">
       <c r="A34" s="5" t="s">
         <v>54</v>
       </c>
@@ -2419,7 +2476,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8">
       <c r="A35" s="5" t="s">
         <v>118</v>
       </c>
@@ -2436,7 +2493,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8">
       <c r="A36" s="5" t="s">
         <v>172</v>
       </c>
@@ -2456,7 +2513,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8">
       <c r="A37" s="5" t="s">
         <v>189</v>
       </c>
@@ -2476,7 +2533,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8">
       <c r="A38" s="5" t="s">
         <v>55</v>
       </c>
@@ -2493,7 +2550,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8">
       <c r="A39" s="5" t="s">
         <v>15</v>
       </c>
@@ -2510,7 +2567,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8">
       <c r="A40" s="5" t="s">
         <v>19</v>
       </c>
@@ -2527,7 +2584,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8">
       <c r="A41" s="5" t="s">
         <v>62</v>
       </c>
@@ -2544,7 +2601,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8">
       <c r="A42" s="5" t="s">
         <v>196</v>
       </c>
@@ -2561,7 +2618,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8">
       <c r="A43" s="5" t="s">
         <v>69</v>
       </c>
@@ -2578,7 +2635,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8">
       <c r="A44" s="5" t="s">
         <v>86</v>
       </c>
@@ -2595,7 +2652,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8">
       <c r="A45" s="5" t="s">
         <v>143</v>
       </c>
@@ -2612,7 +2669,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8">
       <c r="A46" s="5" t="s">
         <v>199</v>
       </c>
@@ -2629,7 +2686,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8">
       <c r="A47" s="5" t="s">
         <v>20</v>
       </c>
@@ -2646,7 +2703,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8">
       <c r="A48" s="5" t="s">
         <v>123</v>
       </c>
@@ -2663,7 +2720,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8">
       <c r="A49" s="5" t="s">
         <v>70</v>
       </c>
@@ -2680,7 +2737,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8">
       <c r="A50" s="5" t="s">
         <v>56</v>
       </c>
@@ -2697,7 +2754,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8">
       <c r="A51" s="5" t="s">
         <v>203</v>
       </c>
@@ -2714,7 +2771,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8">
       <c r="A52" s="5" t="s">
         <v>63</v>
       </c>
@@ -2731,7 +2788,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8">
       <c r="A53" s="5" t="s">
         <v>21</v>
       </c>
@@ -2748,7 +2805,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" ht="43">
       <c r="A54" s="5" t="s">
         <v>22</v>
       </c>
@@ -2771,7 +2828,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8">
       <c r="A55" s="5" t="s">
         <v>191</v>
       </c>
@@ -2788,7 +2845,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8">
       <c r="A56" s="5" t="s">
         <v>165</v>
       </c>
@@ -2805,7 +2862,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8">
       <c r="A57" s="5" t="s">
         <v>152</v>
       </c>
@@ -2822,7 +2879,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8">
       <c r="A58" s="5" t="s">
         <v>134</v>
       </c>
@@ -2839,7 +2896,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8">
       <c r="A59" s="5" t="s">
         <v>124</v>
       </c>
@@ -2862,7 +2919,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8">
       <c r="A60" s="5" t="s">
         <v>78</v>
       </c>
@@ -2879,7 +2936,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8">
       <c r="A61" s="5" t="s">
         <v>23</v>
       </c>
@@ -2896,7 +2953,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8">
       <c r="A62" s="5" t="s">
         <v>16</v>
       </c>
@@ -2913,7 +2970,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8">
       <c r="A63" s="5" t="s">
         <v>183</v>
       </c>
@@ -2930,7 +2987,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8">
       <c r="A64" s="5" t="s">
         <v>24</v>
       </c>
@@ -2947,7 +3004,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7">
       <c r="A65" s="5" t="s">
         <v>204</v>
       </c>
@@ -2964,7 +3021,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7">
       <c r="A66" s="5" t="s">
         <v>175</v>
       </c>
@@ -2981,7 +3038,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7">
       <c r="A67" s="5" t="s">
         <v>144</v>
       </c>
@@ -2998,7 +3055,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7">
       <c r="A68" s="5" t="s">
         <v>125</v>
       </c>
@@ -3015,7 +3072,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7">
       <c r="A69" s="5" t="s">
         <v>25</v>
       </c>
@@ -3032,7 +3089,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7">
       <c r="A70" s="5" t="s">
         <v>139</v>
       </c>
@@ -3049,7 +3106,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7">
       <c r="A71" s="5" t="s">
         <v>153</v>
       </c>
@@ -3066,7 +3123,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7">
       <c r="A72" s="5" t="s">
         <v>126</v>
       </c>
@@ -3083,7 +3140,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7">
       <c r="A73" s="5" t="s">
         <v>161</v>
       </c>
@@ -3100,7 +3157,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7">
       <c r="A74" s="5" t="s">
         <v>71</v>
       </c>
@@ -3117,7 +3174,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7">
       <c r="A75" s="5" t="s">
         <v>64</v>
       </c>
@@ -3134,7 +3191,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7">
       <c r="A76" s="5" t="s">
         <v>26</v>
       </c>
@@ -3151,7 +3208,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7">
       <c r="A77" s="5" t="s">
         <v>79</v>
       </c>
@@ -3168,7 +3225,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7">
       <c r="A78" s="5" t="s">
         <v>72</v>
       </c>
@@ -3185,7 +3242,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7">
       <c r="A79" s="5" t="s">
         <v>65</v>
       </c>
@@ -3202,7 +3259,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7">
       <c r="A80" s="5" t="s">
         <v>105</v>
       </c>
@@ -3219,7 +3276,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8">
       <c r="A81" s="5" t="s">
         <v>145</v>
       </c>
@@ -3236,7 +3293,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8">
       <c r="A82" s="5" t="s">
         <v>135</v>
       </c>
@@ -3253,7 +3310,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8">
       <c r="A83" s="5" t="s">
         <v>106</v>
       </c>
@@ -3270,7 +3327,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8">
       <c r="A84" s="5" t="s">
         <v>107</v>
       </c>
@@ -3287,7 +3344,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8">
       <c r="A85" s="5" t="s">
         <v>87</v>
       </c>
@@ -3304,7 +3361,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8">
       <c r="A86" s="5" t="s">
         <v>88</v>
       </c>
@@ -3321,7 +3378,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8">
       <c r="A87" s="5" t="s">
         <v>127</v>
       </c>
@@ -3338,7 +3395,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8">
       <c r="A88" s="5" t="s">
         <v>83</v>
       </c>
@@ -3355,7 +3412,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8">
       <c r="A89" s="5" t="s">
         <v>128</v>
       </c>
@@ -3378,7 +3435,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8">
       <c r="A90" s="5" t="s">
         <v>27</v>
       </c>
@@ -3395,7 +3452,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:8">
       <c r="A91" s="5" t="s">
         <v>73</v>
       </c>
@@ -3412,7 +3469,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8">
       <c r="A92" s="5" t="s">
         <v>84</v>
       </c>
@@ -3429,7 +3486,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8">
       <c r="A93" s="5" t="s">
         <v>184</v>
       </c>
@@ -3446,7 +3503,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8">
       <c r="A94" s="5" t="s">
         <v>89</v>
       </c>
@@ -3463,7 +3520,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8">
       <c r="A95" s="5" t="s">
         <v>28</v>
       </c>
@@ -3480,7 +3537,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8">
       <c r="A96" s="5" t="s">
         <v>119</v>
       </c>
@@ -3497,7 +3554,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6">
       <c r="A97" s="5" t="s">
         <v>108</v>
       </c>
@@ -3514,7 +3571,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6">
       <c r="A98" s="5" t="s">
         <v>90</v>
       </c>
@@ -3531,7 +3588,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6">
       <c r="A99" s="5" t="s">
         <v>185</v>
       </c>
@@ -3548,7 +3605,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6">
       <c r="A100" s="5" t="s">
         <v>109</v>
       </c>
@@ -3565,7 +3622,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6">
       <c r="A101" s="5" t="s">
         <v>91</v>
       </c>
@@ -3582,7 +3639,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6">
       <c r="A102" s="5" t="s">
         <v>192</v>
       </c>
@@ -3599,7 +3656,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6">
       <c r="A103" s="5" t="s">
         <v>29</v>
       </c>
@@ -3616,7 +3673,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6">
       <c r="A104" s="5" t="s">
         <v>7</v>
       </c>
@@ -3633,7 +3690,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6">
       <c r="A105" s="5" t="s">
         <v>193</v>
       </c>
@@ -3650,7 +3707,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6">
       <c r="A106" s="5" t="s">
         <v>110</v>
       </c>
@@ -3667,7 +3724,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6">
       <c r="A107" s="5" t="s">
         <v>30</v>
       </c>
@@ -3684,7 +3741,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6">
       <c r="A108" s="5" t="s">
         <v>158</v>
       </c>
@@ -3701,7 +3758,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6">
       <c r="A109" s="5" t="s">
         <v>111</v>
       </c>
@@ -3718,7 +3775,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6">
       <c r="A110" s="5" t="s">
         <v>31</v>
       </c>
@@ -3735,7 +3792,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6">
       <c r="A111" s="5" t="s">
         <v>140</v>
       </c>
@@ -3752,7 +3809,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6">
       <c r="A112" s="5" t="s">
         <v>32</v>
       </c>
@@ -3769,7 +3826,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6">
       <c r="A113" s="5" t="s">
         <v>33</v>
       </c>
@@ -3786,7 +3843,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6">
       <c r="A114" s="5" t="s">
         <v>57</v>
       </c>
@@ -3803,7 +3860,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6">
       <c r="A115" s="5" t="s">
         <v>120</v>
       </c>
@@ -3820,7 +3877,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6">
       <c r="A116" s="5" t="s">
         <v>194</v>
       </c>
@@ -3837,7 +3894,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6">
       <c r="A117" s="5" t="s">
         <v>8</v>
       </c>
@@ -3854,7 +3911,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6">
       <c r="A118" s="5" t="s">
         <v>34</v>
       </c>
@@ -3871,7 +3928,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6">
       <c r="A119" s="5" t="s">
         <v>92</v>
       </c>
@@ -3888,7 +3945,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6">
       <c r="A120" s="5" t="s">
         <v>112</v>
       </c>
@@ -3905,7 +3962,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6">
       <c r="A121" s="5" t="s">
         <v>129</v>
       </c>
@@ -3922,7 +3979,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6">
       <c r="A122" s="5" t="s">
         <v>74</v>
       </c>
@@ -3939,7 +3996,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6">
       <c r="A123" s="5" t="s">
         <v>166</v>
       </c>
@@ -3956,7 +4013,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6">
       <c r="A124" s="5" t="s">
         <v>154</v>
       </c>
@@ -3973,7 +4030,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6">
       <c r="A125" s="5" t="s">
         <v>151</v>
       </c>
@@ -3990,7 +4047,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6">
       <c r="A126" s="5" t="s">
         <v>66</v>
       </c>
@@ -4007,7 +4064,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6">
       <c r="A127" s="5" t="s">
         <v>35</v>
       </c>
@@ -4024,7 +4081,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6">
       <c r="A128" s="5" t="s">
         <v>36</v>
       </c>
@@ -4041,7 +4098,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:8">
       <c r="A129" s="5" t="s">
         <v>136</v>
       </c>
@@ -4055,7 +4112,7 @@
         <v>249</v>
       </c>
       <c r="F129" s="11" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="G129" s="3" t="s">
         <v>446</v>
@@ -4064,7 +4121,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:8">
       <c r="A130" s="5" t="s">
         <v>113</v>
       </c>
@@ -4081,7 +4138,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:8">
       <c r="A131" s="5" t="s">
         <v>80</v>
       </c>
@@ -4101,7 +4158,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:8">
       <c r="A132" s="5" t="s">
         <v>155</v>
       </c>
@@ -4118,7 +4175,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:8">
       <c r="A133" s="5" t="s">
         <v>58</v>
       </c>
@@ -4135,7 +4192,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:8">
       <c r="A134" s="5" t="s">
         <v>59</v>
       </c>
@@ -4152,7 +4209,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:8">
       <c r="A135" s="5" t="s">
         <v>114</v>
       </c>
@@ -4169,7 +4226,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:8">
       <c r="A136" s="5" t="s">
         <v>146</v>
       </c>
@@ -4186,7 +4243,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:8">
       <c r="A137" s="5" t="s">
         <v>130</v>
       </c>
@@ -4203,7 +4260,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:8">
       <c r="A138" s="5" t="s">
         <v>37</v>
       </c>
@@ -4220,7 +4277,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:8">
       <c r="A139" s="5" t="s">
         <v>93</v>
       </c>
@@ -4237,7 +4294,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:8">
       <c r="A140" s="5" t="s">
         <v>38</v>
       </c>
@@ -4257,7 +4314,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:8">
       <c r="A141" s="5" t="s">
         <v>147</v>
       </c>
@@ -4274,7 +4331,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:8">
       <c r="A142" s="5" t="s">
         <v>176</v>
       </c>
@@ -4291,7 +4348,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:8">
       <c r="A143" s="5" t="s">
         <v>159</v>
       </c>
@@ -4308,7 +4365,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:8">
       <c r="A144" s="5" t="s">
         <v>163</v>
       </c>
@@ -4325,7 +4382,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:6">
       <c r="A145" s="5" t="s">
         <v>75</v>
       </c>
@@ -4342,7 +4399,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6">
       <c r="A146" s="5" t="s">
         <v>50</v>
       </c>
@@ -4359,7 +4416,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:6">
       <c r="A147" s="5" t="s">
         <v>94</v>
       </c>
@@ -4376,7 +4433,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:6">
       <c r="A148" s="5" t="s">
         <v>39</v>
       </c>
@@ -4393,7 +4450,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:6">
       <c r="A149" s="5" t="s">
         <v>162</v>
       </c>
@@ -4410,7 +4467,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:6">
       <c r="A150" s="5" t="s">
         <v>40</v>
       </c>
@@ -4427,7 +4484,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:6">
       <c r="A151" s="5" t="s">
         <v>115</v>
       </c>
@@ -4444,7 +4501,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:6">
       <c r="A152" s="5" t="s">
         <v>180</v>
       </c>
@@ -4461,7 +4518,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:6">
       <c r="A153" s="5" t="s">
         <v>121</v>
       </c>
@@ -4478,7 +4535,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:6">
       <c r="A154" s="5" t="s">
         <v>197</v>
       </c>
@@ -4495,7 +4552,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:6">
       <c r="A155" s="5" t="s">
         <v>41</v>
       </c>
@@ -4512,7 +4569,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:6">
       <c r="A156" s="5" t="s">
         <v>5</v>
       </c>
@@ -4529,7 +4586,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:6">
       <c r="A157" s="5" t="s">
         <v>160</v>
       </c>
@@ -4546,7 +4603,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:6">
       <c r="A158" s="5" t="s">
         <v>95</v>
       </c>
@@ -4563,7 +4620,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:6">
       <c r="A159" s="5" t="s">
         <v>131</v>
       </c>
@@ -4580,7 +4637,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:6">
       <c r="A160" s="5" t="s">
         <v>9</v>
       </c>
@@ -4597,7 +4654,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:8">
       <c r="A161" s="5" t="s">
         <v>81</v>
       </c>
@@ -4614,7 +4671,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:8">
       <c r="A162" s="5" t="s">
         <v>137</v>
       </c>
@@ -4631,7 +4688,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:8">
       <c r="A163" s="5" t="s">
         <v>138</v>
       </c>
@@ -4654,7 +4711,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:8">
       <c r="A164" s="5" t="s">
         <v>96</v>
       </c>
@@ -4671,7 +4728,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:8">
       <c r="A165" s="5" t="s">
         <v>186</v>
       </c>
@@ -4688,7 +4745,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:8">
       <c r="A166" s="5" t="s">
         <v>116</v>
       </c>
@@ -4705,7 +4762,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:8">
       <c r="A167" s="5" t="s">
         <v>42</v>
       </c>
@@ -4722,7 +4779,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:8">
       <c r="A168" s="5" t="s">
         <v>76</v>
       </c>
@@ -4739,7 +4796,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:8">
       <c r="A169" s="5" t="s">
         <v>97</v>
       </c>
@@ -4756,7 +4813,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:8">
       <c r="A170" s="5" t="s">
         <v>10</v>
       </c>
@@ -4773,7 +4830,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:8">
       <c r="A171" s="5" t="s">
         <v>98</v>
       </c>
@@ -4790,7 +4847,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:8">
       <c r="A172" s="5" t="s">
         <v>187</v>
       </c>
@@ -4807,7 +4864,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:8">
       <c r="A173" s="5" t="s">
         <v>43</v>
       </c>
@@ -4824,7 +4881,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:8">
       <c r="A174" s="5" t="s">
         <v>177</v>
       </c>
@@ -4841,7 +4898,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:8">
       <c r="A175" s="5" t="s">
         <v>200</v>
       </c>
@@ -4858,7 +4915,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:8">
       <c r="A176" s="5" t="s">
         <v>149</v>
       </c>
@@ -4875,7 +4932,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:8">
       <c r="A177" s="5" t="s">
         <v>11</v>
       </c>
@@ -4892,7 +4949,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:8">
       <c r="A178" s="5" t="s">
         <v>132</v>
       </c>
@@ -4909,7 +4966,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:8">
       <c r="A179" s="5" t="s">
         <v>44</v>
       </c>
@@ -4926,7 +4983,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:8">
       <c r="A180" s="5" t="s">
         <v>48</v>
       </c>
@@ -4949,7 +5006,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:8">
       <c r="A181" s="5" t="s">
         <v>45</v>
       </c>
@@ -4966,7 +5023,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:8">
       <c r="A182" s="5" t="s">
         <v>60</v>
       </c>
@@ -4983,7 +5040,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:8">
       <c r="A183" s="5" t="s">
         <v>188</v>
       </c>
@@ -5000,7 +5057,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:8">
       <c r="A184" s="5" t="s">
         <v>61</v>
       </c>
@@ -5017,7 +5074,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:8">
       <c r="A185" s="5" t="s">
         <v>169</v>
       </c>
@@ -5034,7 +5091,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:8">
       <c r="A186" s="5" t="s">
         <v>99</v>
       </c>
@@ -5051,7 +5108,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:8">
       <c r="A187" s="5" t="s">
         <v>179</v>
       </c>
@@ -5068,7 +5125,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:8">
       <c r="A188" s="5" t="s">
         <v>156</v>
       </c>
@@ -5082,7 +5139,7 @@
         <v>249</v>
       </c>
       <c r="F188" s="11" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="G188" s="3" t="s">
         <v>455</v>
@@ -5091,7 +5148,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:8">
       <c r="A189" s="5" t="s">
         <v>148</v>
       </c>
@@ -5108,7 +5165,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:8">
       <c r="A190" s="5" t="s">
         <v>178</v>
       </c>
@@ -5125,7 +5182,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:8">
       <c r="A191" s="5" t="s">
         <v>46</v>
       </c>
@@ -5142,7 +5199,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:8">
       <c r="A192" s="5" t="s">
         <v>82</v>
       </c>
@@ -5159,7 +5216,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:8">
       <c r="A193" s="5" t="s">
         <v>117</v>
       </c>
@@ -5182,7 +5239,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:8">
       <c r="A194" s="5" t="s">
         <v>157</v>
       </c>
@@ -5199,7 +5256,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:8">
       <c r="A195" s="5" t="s">
         <v>168</v>
       </c>
@@ -5216,7 +5273,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:8">
       <c r="A196" s="5" t="s">
         <v>170</v>
       </c>
@@ -5233,7 +5290,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:8">
       <c r="A197" s="5" t="s">
         <v>171</v>
       </c>
@@ -5250,7 +5307,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:8">
       <c r="A198" s="5" t="s">
         <v>173</v>
       </c>
@@ -5267,7 +5324,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:8">
       <c r="A199" s="5" t="s">
         <v>174</v>
       </c>
@@ -5284,7 +5341,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:8">
       <c r="A200" s="5" t="s">
         <v>198</v>
       </c>
@@ -5301,7 +5358,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:8">
       <c r="A201" s="5" t="s">
         <v>201</v>
       </c>
@@ -5318,7 +5375,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:8">
       <c r="A202" s="5" t="s">
         <v>202</v>
       </c>
@@ -5340,5 +5397,11 @@
     <sortCondition ref="C2:C202"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added comment about YEMEN but is accounted for in intertemporal coding of country adjustments
</commit_message>
<xml_diff>
--- a/pyeconlab/trade/dataset/NBERFeenstraWTF/checks/check_exporters.xlsx
+++ b/pyeconlab/trade/dataset/NBERFeenstraWTF/checks/check_exporters.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24816"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="80" windowWidth="16100" windowHeight="9600"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="16095" windowHeight="9600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="457">
   <si>
     <t>exporter</t>
   </si>
@@ -1408,6 +1408,9 @@
   </si>
   <si>
     <t>Recode to 882, 'WSM'</t>
+  </si>
+  <si>
+    <t>Should this be recoded to YEM?</t>
   </si>
 </sst>
 </file>
@@ -1866,24 +1869,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="F180" sqref="F180:H180"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="H188" sqref="H188"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="2"/>
-    <col min="6" max="6" width="9.6640625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="35.1640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="70.5" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="2"/>
+    <col min="6" max="6" width="16.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="70.42578125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1906,7 +1909,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1923,7 +1926,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>100</v>
       </c>
@@ -1946,7 +1949,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>101</v>
       </c>
@@ -1966,7 +1969,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>141</v>
       </c>
@@ -1983,7 +1986,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -2000,7 +2003,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
@@ -2017,7 +2020,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>181</v>
       </c>
@@ -2034,7 +2037,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>51</v>
       </c>
@@ -2051,7 +2054,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>150</v>
       </c>
@@ -2068,7 +2071,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>133</v>
       </c>
@@ -2085,7 +2088,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>67</v>
       </c>
@@ -2102,7 +2105,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>85</v>
       </c>
@@ -2119,7 +2122,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>167</v>
       </c>
@@ -2136,7 +2139,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>182</v>
       </c>
@@ -2153,7 +2156,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>68</v>
       </c>
@@ -2170,7 +2173,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>122</v>
       </c>
@@ -2187,7 +2190,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>49</v>
       </c>
@@ -2204,7 +2207,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>52</v>
       </c>
@@ -2221,7 +2224,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>195</v>
       </c>
@@ -2238,7 +2241,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>53</v>
       </c>
@@ -2255,7 +2258,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>164</v>
       </c>
@@ -2272,7 +2275,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>77</v>
       </c>
@@ -2289,7 +2292,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>142</v>
       </c>
@@ -2306,7 +2309,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>102</v>
       </c>
@@ -2323,7 +2326,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>18</v>
       </c>
@@ -2340,7 +2343,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>190</v>
       </c>
@@ -2357,7 +2360,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>103</v>
       </c>
@@ -2374,7 +2377,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>12</v>
       </c>
@@ -2391,7 +2394,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>47</v>
       </c>
@@ -2408,7 +2411,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>13</v>
       </c>
@@ -2425,7 +2428,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>104</v>
       </c>
@@ -2442,7 +2445,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>14</v>
       </c>
@@ -2459,7 +2462,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>54</v>
       </c>
@@ -2476,7 +2479,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>118</v>
       </c>
@@ -2493,7 +2496,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>172</v>
       </c>
@@ -2513,7 +2516,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>189</v>
       </c>
@@ -2533,7 +2536,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>55</v>
       </c>
@@ -2550,7 +2553,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>15</v>
       </c>
@@ -2567,7 +2570,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>19</v>
       </c>
@@ -2584,7 +2587,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>62</v>
       </c>
@@ -2601,7 +2604,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>196</v>
       </c>
@@ -2618,7 +2621,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>69</v>
       </c>
@@ -2635,7 +2638,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>86</v>
       </c>
@@ -2652,7 +2655,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>143</v>
       </c>
@@ -2669,7 +2672,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>199</v>
       </c>
@@ -2686,7 +2689,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>20</v>
       </c>
@@ -2703,7 +2706,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>123</v>
       </c>
@@ -2720,7 +2723,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>70</v>
       </c>
@@ -2737,7 +2740,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>56</v>
       </c>
@@ -2754,7 +2757,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>203</v>
       </c>
@@ -2771,7 +2774,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>63</v>
       </c>
@@ -2788,7 +2791,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>21</v>
       </c>
@@ -2805,7 +2808,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="43">
+    <row r="54" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>22</v>
       </c>
@@ -2828,7 +2831,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>191</v>
       </c>
@@ -2845,7 +2848,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>165</v>
       </c>
@@ -2862,7 +2865,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>152</v>
       </c>
@@ -2879,7 +2882,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>134</v>
       </c>
@@ -2896,7 +2899,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>124</v>
       </c>
@@ -2919,7 +2922,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>78</v>
       </c>
@@ -2936,7 +2939,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>23</v>
       </c>
@@ -2953,7 +2956,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>16</v>
       </c>
@@ -2970,7 +2973,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>183</v>
       </c>
@@ -2987,7 +2990,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>24</v>
       </c>
@@ -3004,7 +3007,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>204</v>
       </c>
@@ -3021,7 +3024,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>175</v>
       </c>
@@ -3038,7 +3041,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
         <v>144</v>
       </c>
@@ -3055,7 +3058,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>125</v>
       </c>
@@ -3072,7 +3075,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>25</v>
       </c>
@@ -3089,7 +3092,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>139</v>
       </c>
@@ -3106,7 +3109,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
         <v>153</v>
       </c>
@@ -3123,7 +3126,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>126</v>
       </c>
@@ -3140,7 +3143,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
         <v>161</v>
       </c>
@@ -3157,7 +3160,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
         <v>71</v>
       </c>
@@ -3174,7 +3177,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>64</v>
       </c>
@@ -3191,7 +3194,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>26</v>
       </c>
@@ -3208,7 +3211,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
         <v>79</v>
       </c>
@@ -3225,7 +3228,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>72</v>
       </c>
@@ -3242,7 +3245,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>65</v>
       </c>
@@ -3259,7 +3262,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
         <v>105</v>
       </c>
@@ -3276,7 +3279,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
         <v>145</v>
       </c>
@@ -3293,7 +3296,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
         <v>135</v>
       </c>
@@ -3310,7 +3313,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
         <v>106</v>
       </c>
@@ -3327,7 +3330,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
         <v>107</v>
       </c>
@@ -3344,7 +3347,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>87</v>
       </c>
@@ -3361,7 +3364,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>88</v>
       </c>
@@ -3378,7 +3381,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
         <v>127</v>
       </c>
@@ -3395,7 +3398,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>83</v>
       </c>
@@ -3412,7 +3415,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>128</v>
       </c>
@@ -3435,7 +3438,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>27</v>
       </c>
@@ -3452,7 +3455,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
         <v>73</v>
       </c>
@@ -3469,7 +3472,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>84</v>
       </c>
@@ -3486,7 +3489,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
         <v>184</v>
       </c>
@@ -3503,7 +3506,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
         <v>89</v>
       </c>
@@ -3520,7 +3523,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
         <v>28</v>
       </c>
@@ -3537,7 +3540,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
         <v>119</v>
       </c>
@@ -3554,7 +3557,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
         <v>108</v>
       </c>
@@ -3571,7 +3574,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="5" t="s">
         <v>90</v>
       </c>
@@ -3588,7 +3591,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
         <v>185</v>
       </c>
@@ -3605,7 +3608,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
         <v>109</v>
       </c>
@@ -3622,7 +3625,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
         <v>91</v>
       </c>
@@ -3639,7 +3642,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>192</v>
       </c>
@@ -3656,7 +3659,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
         <v>29</v>
       </c>
@@ -3673,7 +3676,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
         <v>7</v>
       </c>
@@ -3690,7 +3693,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" s="5" t="s">
         <v>193</v>
       </c>
@@ -3707,7 +3710,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
         <v>110</v>
       </c>
@@ -3724,7 +3727,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
         <v>30</v>
       </c>
@@ -3741,7 +3744,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
         <v>158</v>
       </c>
@@ -3758,7 +3761,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
         <v>111</v>
       </c>
@@ -3775,7 +3778,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
         <v>31</v>
       </c>
@@ -3792,7 +3795,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" s="5" t="s">
         <v>140</v>
       </c>
@@ -3809,7 +3812,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
         <v>32</v>
       </c>
@@ -3826,7 +3829,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" s="5" t="s">
         <v>33</v>
       </c>
@@ -3843,7 +3846,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" s="5" t="s">
         <v>57</v>
       </c>
@@ -3860,7 +3863,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" s="5" t="s">
         <v>120</v>
       </c>
@@ -3877,7 +3880,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" s="5" t="s">
         <v>194</v>
       </c>
@@ -3894,7 +3897,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" s="5" t="s">
         <v>8</v>
       </c>
@@ -3911,7 +3914,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" s="5" t="s">
         <v>34</v>
       </c>
@@ -3928,7 +3931,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" s="5" t="s">
         <v>92</v>
       </c>
@@ -3945,7 +3948,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" s="5" t="s">
         <v>112</v>
       </c>
@@ -3962,7 +3965,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" s="5" t="s">
         <v>129</v>
       </c>
@@ -3979,7 +3982,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" s="5" t="s">
         <v>74</v>
       </c>
@@ -3996,7 +3999,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" s="5" t="s">
         <v>166</v>
       </c>
@@ -4013,7 +4016,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" s="5" t="s">
         <v>154</v>
       </c>
@@ -4030,7 +4033,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" s="5" t="s">
         <v>151</v>
       </c>
@@ -4047,7 +4050,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" s="5" t="s">
         <v>66</v>
       </c>
@@ -4064,7 +4067,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" s="5" t="s">
         <v>35</v>
       </c>
@@ -4081,7 +4084,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" s="5" t="s">
         <v>36</v>
       </c>
@@ -4098,7 +4101,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" s="5" t="s">
         <v>136</v>
       </c>
@@ -4121,7 +4124,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" s="5" t="s">
         <v>113</v>
       </c>
@@ -4138,7 +4141,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" s="5" t="s">
         <v>80</v>
       </c>
@@ -4158,7 +4161,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" s="5" t="s">
         <v>155</v>
       </c>
@@ -4175,7 +4178,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" s="5" t="s">
         <v>58</v>
       </c>
@@ -4192,7 +4195,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" s="5" t="s">
         <v>59</v>
       </c>
@@ -4209,7 +4212,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" s="5" t="s">
         <v>114</v>
       </c>
@@ -4226,7 +4229,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" s="5" t="s">
         <v>146</v>
       </c>
@@ -4243,7 +4246,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" s="5" t="s">
         <v>130</v>
       </c>
@@ -4260,7 +4263,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" s="5" t="s">
         <v>37</v>
       </c>
@@ -4277,7 +4280,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139" s="5" t="s">
         <v>93</v>
       </c>
@@ -4294,7 +4297,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A140" s="5" t="s">
         <v>38</v>
       </c>
@@ -4314,7 +4317,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A141" s="5" t="s">
         <v>147</v>
       </c>
@@ -4331,7 +4334,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A142" s="5" t="s">
         <v>176</v>
       </c>
@@ -4348,7 +4351,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A143" s="5" t="s">
         <v>159</v>
       </c>
@@ -4365,7 +4368,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A144" s="5" t="s">
         <v>163</v>
       </c>
@@ -4382,7 +4385,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145" s="5" t="s">
         <v>75</v>
       </c>
@@ -4399,7 +4402,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146" s="5" t="s">
         <v>50</v>
       </c>
@@ -4416,7 +4419,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A147" s="5" t="s">
         <v>94</v>
       </c>
@@ -4433,7 +4436,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A148" s="5" t="s">
         <v>39</v>
       </c>
@@ -4450,7 +4453,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149" s="5" t="s">
         <v>162</v>
       </c>
@@ -4467,7 +4470,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150" s="5" t="s">
         <v>40</v>
       </c>
@@ -4484,7 +4487,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151" s="5" t="s">
         <v>115</v>
       </c>
@@ -4501,7 +4504,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A152" s="5" t="s">
         <v>180</v>
       </c>
@@ -4518,7 +4521,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A153" s="5" t="s">
         <v>121</v>
       </c>
@@ -4535,7 +4538,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="154" spans="1:6">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A154" s="5" t="s">
         <v>197</v>
       </c>
@@ -4552,7 +4555,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="155" spans="1:6">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A155" s="5" t="s">
         <v>41</v>
       </c>
@@ -4569,7 +4572,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="156" spans="1:6">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A156" s="5" t="s">
         <v>5</v>
       </c>
@@ -4586,7 +4589,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="157" spans="1:6">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A157" s="5" t="s">
         <v>160</v>
       </c>
@@ -4603,7 +4606,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="158" spans="1:6">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A158" s="5" t="s">
         <v>95</v>
       </c>
@@ -4619,8 +4622,11 @@
       <c r="F158" s="11" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="159" spans="1:6">
+      <c r="H158" s="2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A159" s="5" t="s">
         <v>131</v>
       </c>
@@ -4637,7 +4643,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="160" spans="1:6">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A160" s="5" t="s">
         <v>9</v>
       </c>
@@ -4654,7 +4660,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A161" s="5" t="s">
         <v>81</v>
       </c>
@@ -4671,7 +4677,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A162" s="5" t="s">
         <v>137</v>
       </c>
@@ -4688,7 +4694,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" s="5" t="s">
         <v>138</v>
       </c>
@@ -4711,7 +4717,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" s="5" t="s">
         <v>96</v>
       </c>
@@ -4728,7 +4734,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A165" s="5" t="s">
         <v>186</v>
       </c>
@@ -4745,7 +4751,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A166" s="5" t="s">
         <v>116</v>
       </c>
@@ -4762,7 +4768,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A167" s="5" t="s">
         <v>42</v>
       </c>
@@ -4779,7 +4785,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A168" s="5" t="s">
         <v>76</v>
       </c>
@@ -4796,7 +4802,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A169" s="5" t="s">
         <v>97</v>
       </c>
@@ -4813,7 +4819,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A170" s="5" t="s">
         <v>10</v>
       </c>
@@ -4830,7 +4836,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171" s="5" t="s">
         <v>98</v>
       </c>
@@ -4847,7 +4853,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A172" s="5" t="s">
         <v>187</v>
       </c>
@@ -4864,7 +4870,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A173" s="5" t="s">
         <v>43</v>
       </c>
@@ -4881,7 +4887,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="174" spans="1:8">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A174" s="5" t="s">
         <v>177</v>
       </c>
@@ -4898,7 +4904,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A175" s="5" t="s">
         <v>200</v>
       </c>
@@ -4915,7 +4921,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A176" s="5" t="s">
         <v>149</v>
       </c>
@@ -4932,7 +4938,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A177" s="5" t="s">
         <v>11</v>
       </c>
@@ -4949,7 +4955,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="178" spans="1:8">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A178" s="5" t="s">
         <v>132</v>
       </c>
@@ -4966,7 +4972,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="179" spans="1:8">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A179" s="5" t="s">
         <v>44</v>
       </c>
@@ -4983,7 +4989,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="180" spans="1:8">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A180" s="5" t="s">
         <v>48</v>
       </c>
@@ -5006,7 +5012,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="181" spans="1:8">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A181" s="5" t="s">
         <v>45</v>
       </c>
@@ -5023,7 +5029,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A182" s="5" t="s">
         <v>60</v>
       </c>
@@ -5040,7 +5046,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A183" s="5" t="s">
         <v>188</v>
       </c>
@@ -5057,7 +5063,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A184" s="5" t="s">
         <v>61</v>
       </c>
@@ -5074,7 +5080,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A185" s="5" t="s">
         <v>169</v>
       </c>
@@ -5091,7 +5097,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="186" spans="1:8">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A186" s="5" t="s">
         <v>99</v>
       </c>
@@ -5107,8 +5113,11 @@
       <c r="F186" s="11" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="187" spans="1:8">
+      <c r="H186" s="2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A187" s="5" t="s">
         <v>179</v>
       </c>
@@ -5125,7 +5134,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="188" spans="1:8">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A188" s="5" t="s">
         <v>156</v>
       </c>
@@ -5148,7 +5157,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="189" spans="1:8">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A189" s="5" t="s">
         <v>148</v>
       </c>
@@ -5165,7 +5174,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="190" spans="1:8">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A190" s="5" t="s">
         <v>178</v>
       </c>
@@ -5182,7 +5191,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="191" spans="1:8">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A191" s="5" t="s">
         <v>46</v>
       </c>
@@ -5199,7 +5208,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="192" spans="1:8">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A192" s="5" t="s">
         <v>82</v>
       </c>
@@ -5216,7 +5225,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="193" spans="1:8">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A193" s="5" t="s">
         <v>117</v>
       </c>
@@ -5239,7 +5248,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="194" spans="1:8">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A194" s="5" t="s">
         <v>157</v>
       </c>
@@ -5256,7 +5265,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="195" spans="1:8">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A195" s="5" t="s">
         <v>168</v>
       </c>
@@ -5273,7 +5282,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="196" spans="1:8">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A196" s="5" t="s">
         <v>170</v>
       </c>
@@ -5290,7 +5299,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="197" spans="1:8">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A197" s="5" t="s">
         <v>171</v>
       </c>
@@ -5307,7 +5316,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="198" spans="1:8">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A198" s="5" t="s">
         <v>173</v>
       </c>
@@ -5324,7 +5333,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="199" spans="1:8">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A199" s="5" t="s">
         <v>174</v>
       </c>
@@ -5341,7 +5350,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="200" spans="1:8">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A200" s="5" t="s">
         <v>198</v>
       </c>
@@ -5358,7 +5367,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="201" spans="1:8">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A201" s="5" t="s">
         <v>201</v>
       </c>
@@ -5375,7 +5384,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="202" spans="1:8">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A202" s="5" t="s">
         <v>202</v>
       </c>

</xml_diff>